<commit_message>
Sectoral advisory board members
</commit_message>
<xml_diff>
--- a/public/indicator1/sectorialboard_members.xlsx
+++ b/public/indicator1/sectorialboard_members.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faith Kilonzi\Documents\ace-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE5FE41-3FC5-45BB-AD1E-0FD57979725A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EC07A7-8443-4311-8413-5871B6F5DDB3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{908C30B9-7C06-4E08-82BD-EF45A389A026}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -151,6 +151,45 @@
   </si>
   <si>
     <t>kilo@kilo.com</t>
+  </si>
+  <si>
+    <t>New Person</t>
+  </si>
+  <si>
+    <t>New position</t>
+  </si>
+  <si>
+    <t>newperson@mail.com</t>
+  </si>
+  <si>
+    <t>New BPerson</t>
+  </si>
+  <si>
+    <t>New C Person</t>
+  </si>
+  <si>
+    <t>New D Person</t>
+  </si>
+  <si>
+    <t>New E Person</t>
+  </si>
+  <si>
+    <t>New F Person</t>
+  </si>
+  <si>
+    <t>newAperson@mail.com</t>
+  </si>
+  <si>
+    <t>newOPerson@mail.com</t>
+  </si>
+  <si>
+    <t>person@mail.com</t>
+  </si>
+  <si>
+    <t>newemali@mail.com</t>
+  </si>
+  <si>
+    <t>testing@mail.com</t>
   </si>
 </sst>
 </file>
@@ -513,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C8798F-292F-4243-B451-A146C70846CF}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,6 +743,90 @@
       </c>
       <c r="D13" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14">
+        <v>780223068</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15">
+        <v>780223069</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>780223070</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17">
+        <v>780223071</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18">
+        <v>780223072</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <v>780223073</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -721,6 +844,12 @@
     <hyperlink ref="D6" r:id="rId11" xr:uid="{7390760C-9380-44E4-93A7-084FDDBB944B}"/>
     <hyperlink ref="D12" r:id="rId12" xr:uid="{F2CF6088-A4C0-4B61-BD80-13FA8D51855A}"/>
     <hyperlink ref="D13" r:id="rId13" xr:uid="{95C25213-88BE-4F4D-B02A-426935010B26}"/>
+    <hyperlink ref="D14" r:id="rId14" xr:uid="{085D2E38-37E3-4B97-94CD-F56A9F83B3A6}"/>
+    <hyperlink ref="D15" r:id="rId15" xr:uid="{AFC5B200-6F18-4DE4-B09C-518434BD3953}"/>
+    <hyperlink ref="D16" r:id="rId16" xr:uid="{C23C6439-CCC9-4481-B71B-AFC77CE927B5}"/>
+    <hyperlink ref="D17" r:id="rId17" xr:uid="{4B8B93AF-A64C-4435-8DD8-2BF67B3C8942}"/>
+    <hyperlink ref="D18" r:id="rId18" xr:uid="{DF7171DC-14AC-4F37-A25D-19BD2B8113BC}"/>
+    <hyperlink ref="D19" r:id="rId19" xr:uid="{FF40A5E3-BF30-4149-8086-EB8029282B41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>